<commit_message>
corregi la data que se cargaba como real, corregi los campos null
</commit_message>
<xml_diff>
--- a/archivos_excel/Base_IPM.xlsx
+++ b/archivos_excel/Base_IPM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/diec_ine_gob_gt/Documents/Escritorio/Cambio de base/Power BI/Bases del tablero extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdpivaral\WebScraping\solucion\archivos_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C6F2784-38A2-4446-8DC4-C084362DD1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66016DC7-2477-4463-8498-A78339CDEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="416">
   <si>
     <t>pais</t>
   </si>
@@ -1172,9 +1172,6 @@
     <t>Elaboración de productos alimenticios</t>
   </si>
   <si>
-    <t>010103122</t>
-  </si>
-  <si>
     <t xml:space="preserve">Agro Industrias Alvarado </t>
   </si>
   <si>
@@ -1184,9 +1181,6 @@
     <t>Abril</t>
   </si>
   <si>
-    <t>010101113</t>
-  </si>
-  <si>
     <t xml:space="preserve">Almacen Cisne Blanco </t>
   </si>
   <si>
@@ -1196,9 +1190,6 @@
     <t>C.14.143.1430</t>
   </si>
   <si>
-    <t>010101011</t>
-  </si>
-  <si>
     <t xml:space="preserve">Almacen Flamingo </t>
   </si>
   <si>
@@ -1208,9 +1199,6 @@
     <t>Marzo</t>
   </si>
   <si>
-    <t>010101073</t>
-  </si>
-  <si>
     <t>Casa Tex</t>
   </si>
   <si>
@@ -1223,45 +1211,30 @@
     <t>Comercio al por menor, excepto el de vehículos automotores y motocicletas</t>
   </si>
   <si>
-    <t>010104124</t>
-  </si>
-  <si>
     <t xml:space="preserve">Disco Centro </t>
   </si>
   <si>
     <t xml:space="preserve">6ta. Avenida 0-60 Local 103 Primer Nivel Centro Comercial Zona 4 </t>
   </si>
   <si>
-    <t>010101120</t>
-  </si>
-  <si>
     <t>Distragsa</t>
   </si>
   <si>
     <t xml:space="preserve">21 calle 11-06 Zona 1 </t>
   </si>
   <si>
-    <t>010101100</t>
-  </si>
-  <si>
     <t xml:space="preserve">El Mundo de las Manualidades </t>
   </si>
   <si>
     <t>9na. Avenida 7-35 Zona 1 Galerías Plaza Local 103</t>
   </si>
   <si>
-    <t>010111036</t>
-  </si>
-  <si>
     <t>El Zeppelin</t>
   </si>
   <si>
     <t xml:space="preserve">16 calle 2-00 zona 10 local 2-33 A centro comercial los Próceres </t>
   </si>
   <si>
-    <t>010101115</t>
-  </si>
-  <si>
     <t>Gx Moda</t>
   </si>
   <si>
@@ -1271,9 +1244,6 @@
     <t>C.25.251.2511</t>
   </si>
   <si>
-    <t>010106118</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herrería Cristián </t>
   </si>
   <si>
@@ -1283,49 +1253,31 @@
     <t>Fabricación de sustancias y productos químicos</t>
   </si>
   <si>
-    <t>010101061</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fragancias del Caribe </t>
   </si>
   <si>
     <t xml:space="preserve">13 Avenida 3-34 Zona 1 </t>
   </si>
   <si>
-    <t>010101114</t>
-  </si>
-  <si>
     <t>Lanquetin</t>
   </si>
   <si>
     <t>10 avenida 4-58 zona 1</t>
   </si>
   <si>
-    <t>010101112</t>
-  </si>
-  <si>
     <t xml:space="preserve">8va. Avenida 11-48 Zona 1 </t>
   </si>
   <si>
     <t>G.47.474.4742</t>
   </si>
   <si>
-    <t>010117123</t>
-  </si>
-  <si>
     <t>Steren</t>
   </si>
   <si>
     <t xml:space="preserve">Km. 5 Carretera al Atlántico Centro Comercial Metro norte Local 2-803 y 2-804 Zona 17 </t>
   </si>
   <si>
-    <t>010101027</t>
-  </si>
-  <si>
     <t>Textiles Cantón</t>
-  </si>
-  <si>
-    <t>010101116</t>
   </si>
   <si>
     <t xml:space="preserve">Zipper </t>
@@ -1341,7 +1293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1375,7 +1327,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1383,7 +1335,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1421,7 +1373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1445,7 +1397,10 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1755,11 +1710,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="N2:O126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1784,7 +1739,7 @@
     <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="23.25" customHeight="1">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1889,10 +1844,10 @@
       <c r="M2" s="3">
         <v>14</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="9">
         <v>14.5874416</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="9">
         <v>-90.514186699999996</v>
       </c>
       <c r="P2" s="3">
@@ -1914,7 +1869,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1954,10 +1909,10 @@
       <c r="M3" s="3">
         <v>9</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="9">
         <v>14.5996793</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="9">
         <v>-90.522157199999995</v>
       </c>
       <c r="P3" s="3">
@@ -1979,7 +1934,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2019,10 +1974,10 @@
       <c r="M4" s="3">
         <v>1</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="9">
         <v>14.6287675</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="9">
         <v>-90.518449599999997</v>
       </c>
       <c r="P4" s="3">
@@ -2044,7 +1999,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2084,10 +2039,10 @@
       <c r="M5" s="3">
         <v>1</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="9">
         <v>14.641237200000001</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="9">
         <v>-90.513992900000005</v>
       </c>
       <c r="P5" s="3">
@@ -2109,7 +2064,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2149,10 +2104,10 @@
       <c r="M6" s="3">
         <v>1</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="9">
         <v>14.626822300000001</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="9">
         <v>-90.520434300000005</v>
       </c>
       <c r="P6" s="3">
@@ -2174,7 +2129,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2214,10 +2169,10 @@
       <c r="M7" s="3">
         <v>1</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="9">
         <v>14.628329600000001</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="9">
         <v>-90.521690899999996</v>
       </c>
       <c r="P7" s="3">
@@ -2239,7 +2194,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2279,10 +2234,10 @@
       <c r="M8" s="3">
         <v>1</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="9">
         <v>14.636915999999999</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="9">
         <v>-90.514626500000006</v>
       </c>
       <c r="P8" s="3">
@@ -2304,7 +2259,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2344,10 +2299,10 @@
       <c r="M9" s="3">
         <v>1</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="9">
         <v>14.640473399999999</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="9">
         <v>-90.508682100000001</v>
       </c>
       <c r="P9" s="3">
@@ -2369,7 +2324,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2409,10 +2364,10 @@
       <c r="M10" s="3">
         <v>1</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="9">
         <v>14.628474499999999</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="9">
         <v>-90.519172499999996</v>
       </c>
       <c r="P10" s="3">
@@ -2434,7 +2389,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2474,10 +2429,10 @@
       <c r="M11" s="3">
         <v>1</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="9">
         <v>14.6428613</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="9">
         <v>-90.511415700000001</v>
       </c>
       <c r="P11" s="3">
@@ -2499,7 +2454,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2539,10 +2494,10 @@
       <c r="M12" s="3">
         <v>1</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="9">
         <v>14.6445344</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="9">
         <v>-90.514564100000001</v>
       </c>
       <c r="P12" s="3">
@@ -2564,7 +2519,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2604,10 +2559,10 @@
       <c r="M13" s="3">
         <v>14</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="9">
         <v>14.5899626</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="9">
         <v>-90.518174200000004</v>
       </c>
       <c r="P13" s="3">
@@ -2629,7 +2584,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2669,10 +2624,10 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="9">
         <v>14.639457500000001</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="9">
         <v>-90.5128792</v>
       </c>
       <c r="P14" s="3">
@@ -2694,7 +2649,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2734,10 +2689,10 @@
       <c r="M15" s="3">
         <v>1</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="9">
         <v>14.641121099999999</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="9">
         <v>-90.510786899999999</v>
       </c>
       <c r="P15" s="3">
@@ -2759,7 +2714,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2799,10 +2754,10 @@
       <c r="M16" s="3">
         <v>4</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="9">
         <v>14.520394400000001</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="9">
         <v>-90.590199900000002</v>
       </c>
       <c r="P16" s="3">
@@ -2824,7 +2779,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2864,10 +2819,10 @@
       <c r="M17" s="3">
         <v>25</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="9">
         <v>14.6365625</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="9">
         <v>-90.423773600000004</v>
       </c>
       <c r="P17" s="3">
@@ -2889,7 +2844,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2929,10 +2884,10 @@
       <c r="M18" s="3">
         <v>4</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="9">
         <v>14.6250698</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="9">
         <v>-90.516529300000002</v>
       </c>
       <c r="P18" s="3">
@@ -2954,7 +2909,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2994,10 +2949,10 @@
       <c r="M19" s="3">
         <v>8</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="9">
         <v>14.6347459</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="9">
         <v>-90.587526400000002</v>
       </c>
       <c r="P19" s="3">
@@ -3019,7 +2974,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -3059,10 +3014,10 @@
       <c r="M20" s="3">
         <v>12</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="9">
         <v>14.5863364</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="9">
         <v>-90.5399259</v>
       </c>
       <c r="P20" s="3">
@@ -3084,7 +3039,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3124,10 +3079,10 @@
       <c r="M21" s="3">
         <v>2</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="9">
         <v>14.5468557</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="9">
         <v>-90.596447299999994</v>
       </c>
       <c r="P21" s="3">
@@ -3149,7 +3104,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3189,10 +3144,10 @@
       <c r="M22" s="3">
         <v>1</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="9">
         <v>14.6397984</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="9">
         <v>-90.511860400000003</v>
       </c>
       <c r="P22" s="3">
@@ -3214,7 +3169,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3254,10 +3209,10 @@
       <c r="M23" s="3">
         <v>1</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="9">
         <v>14.637414700000001</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="9">
         <v>-90.5122961</v>
       </c>
       <c r="P23" s="3">
@@ -3279,7 +3234,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3319,10 +3274,10 @@
       <c r="M24" s="3">
         <v>1</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="9">
         <v>14.640841500000001</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="9">
         <v>-90.511088200000003</v>
       </c>
       <c r="P24" s="3">
@@ -3344,7 +3299,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -3384,10 +3339,10 @@
       <c r="M25" s="3">
         <v>1</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="9">
         <v>14.6406569</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="9">
         <v>-90.509745100000004</v>
       </c>
       <c r="P25" s="3">
@@ -3409,7 +3364,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3449,10 +3404,10 @@
       <c r="M26" s="3">
         <v>1</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="9">
         <v>14.631646</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="9">
         <v>-90.516289900000004</v>
       </c>
       <c r="P26" s="3">
@@ -3474,7 +3429,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3514,10 +3469,10 @@
       <c r="M27" s="3">
         <v>12</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="9">
         <v>14.5946041</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="9">
         <v>-90.537560499999998</v>
       </c>
       <c r="P27" s="3">
@@ -3539,7 +3494,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -3579,10 +3534,10 @@
       <c r="M28" s="3">
         <v>18</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="9">
         <v>14.648084000000001</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="9">
         <v>-90.443537199999994</v>
       </c>
       <c r="P28" s="3">
@@ -3604,7 +3559,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -3644,10 +3599,10 @@
       <c r="M29" s="3">
         <v>3</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="9">
         <v>14.622442100000001</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29" s="9">
         <v>-90.525853400000003</v>
       </c>
       <c r="P29" s="3">
@@ -3669,7 +3624,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -3709,10 +3664,10 @@
       <c r="M30" s="3">
         <v>12</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="9">
         <v>14.5886282</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30" s="9">
         <v>-90.561090899999996</v>
       </c>
       <c r="P30" s="3">
@@ -3734,7 +3689,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -3774,10 +3729,10 @@
       <c r="M31" s="3">
         <v>12</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="9">
         <v>14.5614992</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31" s="9">
         <v>-90.546259199999994</v>
       </c>
       <c r="P31" s="3">
@@ -3799,7 +3754,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -3839,10 +3794,10 @@
       <c r="M32" s="3">
         <v>6</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="9">
         <v>14.6602707</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32" s="9">
         <v>-90.609686100000005</v>
       </c>
       <c r="P32" s="3">
@@ -3864,7 +3819,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -3904,10 +3859,10 @@
       <c r="M33" s="3">
         <v>1</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="9">
         <v>14.6435336</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="9">
         <v>-90.5091982</v>
       </c>
       <c r="P33" s="3">
@@ -3929,7 +3884,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -3969,10 +3924,10 @@
       <c r="M34" s="3">
         <v>12</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="9">
         <v>14.5741636</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34" s="9">
         <v>-90.5424285</v>
       </c>
       <c r="P34" s="3">
@@ -3994,7 +3949,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4034,10 +3989,10 @@
       <c r="M35" s="3">
         <v>4</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="9">
         <v>14.642958399999999</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35" s="9">
         <v>-90.562296700000005</v>
       </c>
       <c r="P35" s="3">
@@ -4059,7 +4014,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -4099,10 +4054,10 @@
       <c r="M36" s="3">
         <v>4</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="9">
         <v>14.5674768</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="9">
         <v>-90.472379000000004</v>
       </c>
       <c r="P36" s="3">
@@ -4124,7 +4079,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -4164,10 +4119,10 @@
       <c r="M37" s="3">
         <v>10</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="9">
         <v>14.6118535</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37" s="9">
         <v>-90.509476899999996</v>
       </c>
       <c r="P37" s="3">
@@ -4189,7 +4144,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -4229,10 +4184,10 @@
       <c r="M38" s="3">
         <v>11</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="9">
         <v>14.5912553</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O38" s="9">
         <v>-90.567270800000003</v>
       </c>
       <c r="P38" s="3">
@@ -4254,7 +4209,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -4294,10 +4249,10 @@
       <c r="M39" s="3">
         <v>17</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="9">
         <v>14.6538892</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39" s="9">
         <v>-90.460154399999993</v>
       </c>
       <c r="P39" s="3">
@@ -4319,7 +4274,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -4359,10 +4314,10 @@
       <c r="M40" s="3">
         <v>8</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="9">
         <v>14.6208998</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40" s="9">
         <v>-90.521817900000002</v>
       </c>
       <c r="P40" s="3">
@@ -4384,7 +4339,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -4424,10 +4379,10 @@
       <c r="M41" s="3">
         <v>4</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="9">
         <v>14.6189958</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41" s="9">
         <v>-90.518116000000006</v>
       </c>
       <c r="P41" s="3">
@@ -4449,7 +4404,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -4489,10 +4444,10 @@
       <c r="M42" s="3">
         <v>7</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="9">
         <v>14.626714</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42" s="9">
         <v>-90.553565699999993</v>
       </c>
       <c r="P42" s="3">
@@ -4514,7 +4469,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -4554,10 +4509,10 @@
       <c r="M43" s="3">
         <v>1</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="9">
         <v>14.6393047</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43" s="9">
         <v>-90.512895200000003</v>
       </c>
       <c r="P43" s="3">
@@ -4579,7 +4534,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -4619,10 +4574,10 @@
       <c r="M44" s="3">
         <v>1</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="9">
         <v>14.644236899999999</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44" s="9">
         <v>-90.504065600000004</v>
       </c>
       <c r="P44" s="3">
@@ -4644,7 +4599,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -4684,10 +4639,10 @@
       <c r="M45" s="3">
         <v>1</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="9">
         <v>14.490701400000001</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45" s="9">
         <v>-90.637698299999997</v>
       </c>
       <c r="P45" s="3">
@@ -4709,7 +4664,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -4749,10 +4704,10 @@
       <c r="M46" s="3">
         <v>1</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="9">
         <v>14.639153500000001</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46" s="9">
         <v>-90.506201599999997</v>
       </c>
       <c r="P46" s="3">
@@ -4774,7 +4729,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -4814,10 +4769,10 @@
       <c r="M47" s="3">
         <v>7</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="9">
         <v>14.621582399999999</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47" s="9">
         <v>-90.547827799999993</v>
       </c>
       <c r="P47" s="3">
@@ -4839,7 +4794,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -4879,10 +4834,10 @@
       <c r="M48" s="3">
         <v>4</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="9">
         <v>14.6168338</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48" s="9">
         <v>-90.515217300000003</v>
       </c>
       <c r="P48" s="3">
@@ -4904,7 +4859,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -4944,10 +4899,10 @@
       <c r="M49" s="3">
         <v>12</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="9">
         <v>14.6046133</v>
       </c>
-      <c r="O49" s="3">
+      <c r="O49" s="9">
         <v>-90.5411565</v>
       </c>
       <c r="P49" s="3">
@@ -4969,7 +4924,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -5009,10 +4964,10 @@
       <c r="M50" s="3">
         <v>1</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="9">
         <v>14.637687700000001</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50" s="9">
         <v>-90.517021200000002</v>
       </c>
       <c r="P50" s="3">
@@ -5034,7 +4989,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -5074,10 +5029,10 @@
       <c r="M51" s="3">
         <v>1</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="9">
         <v>14.6251014</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51" s="9">
         <v>-90.520651400000006</v>
       </c>
       <c r="P51" s="3">
@@ -5099,7 +5054,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
@@ -5139,10 +5094,10 @@
       <c r="M52" s="3">
         <v>2</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="9">
         <v>14.6348208</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O52" s="9">
         <v>-90.595779100000001</v>
       </c>
       <c r="P52" s="3">
@@ -5164,7 +5119,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
@@ -5204,10 +5159,10 @@
       <c r="M53" s="3">
         <v>7</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="9">
         <v>14.6370419</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O53" s="9">
         <v>-90.599217899999999</v>
       </c>
       <c r="P53" s="3">
@@ -5229,7 +5184,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="54" spans="1:21">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -5269,10 +5224,10 @@
       <c r="M54" s="3">
         <v>12</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="9">
         <v>14.564207700000001</v>
       </c>
-      <c r="O54" s="3">
+      <c r="O54" s="9">
         <v>-90.545213799999999</v>
       </c>
       <c r="P54" s="3">
@@ -5294,7 +5249,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -5334,10 +5289,10 @@
       <c r="M55" s="3">
         <v>9</v>
       </c>
-      <c r="N55" s="3">
+      <c r="N55" s="9">
         <v>14.603555500000001</v>
       </c>
-      <c r="O55" s="3">
+      <c r="O55" s="9">
         <v>-90.526756800000001</v>
       </c>
       <c r="P55" s="3">
@@ -5359,7 +5314,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="56" spans="1:21">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -5399,10 +5354,10 @@
       <c r="M56" s="3">
         <v>1</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56" s="9">
         <v>14.6391212</v>
       </c>
-      <c r="O56" s="3">
+      <c r="O56" s="9">
         <v>-90.512805400000005</v>
       </c>
       <c r="P56" s="3">
@@ -5424,7 +5379,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="57" spans="1:21">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -5464,10 +5419,10 @@
       <c r="M57" s="3">
         <v>4</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57" s="9">
         <v>14.6204956</v>
       </c>
-      <c r="O57" s="3">
+      <c r="O57" s="9">
         <v>-90.517846199999994</v>
       </c>
       <c r="P57" s="3">
@@ -5489,7 +5444,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="58" spans="1:21">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -5529,10 +5484,10 @@
       <c r="M58" s="3">
         <v>2</v>
       </c>
-      <c r="N58" s="3">
+      <c r="N58" s="9">
         <v>14.5365194</v>
       </c>
-      <c r="O58" s="3">
+      <c r="O58" s="9">
         <v>-90.586942899999997</v>
       </c>
       <c r="P58" s="3">
@@ -5554,7 +5509,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="59" spans="1:21">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>21</v>
       </c>
@@ -5594,10 +5549,10 @@
       <c r="M59" s="3">
         <v>1</v>
       </c>
-      <c r="N59" s="3">
+      <c r="N59" s="9">
         <v>14.5260569</v>
       </c>
-      <c r="O59" s="3">
+      <c r="O59" s="9">
         <v>-90.595684700000007</v>
       </c>
       <c r="P59" s="3">
@@ -5619,7 +5574,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="60" spans="1:21">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -5659,10 +5614,10 @@
       <c r="M60" s="3">
         <v>10</v>
       </c>
-      <c r="N60" s="3">
+      <c r="N60" s="9">
         <v>14.5983874</v>
       </c>
-      <c r="O60" s="3">
+      <c r="O60" s="9">
         <v>-90.513880599999993</v>
       </c>
       <c r="P60" s="3">
@@ -5684,7 +5639,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>21</v>
       </c>
@@ -5724,10 +5679,10 @@
       <c r="M61" s="3">
         <v>21</v>
       </c>
-      <c r="N61" s="3">
+      <c r="N61" s="9">
         <v>14.5527043</v>
       </c>
-      <c r="O61" s="3">
+      <c r="O61" s="9">
         <v>-90.555820699999998</v>
       </c>
       <c r="P61" s="3">
@@ -5749,7 +5704,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="62" spans="1:21">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>21</v>
       </c>
@@ -5789,10 +5744,10 @@
       <c r="M62" s="3">
         <v>1</v>
       </c>
-      <c r="N62" s="3">
+      <c r="N62" s="9">
         <v>14.6419505</v>
       </c>
-      <c r="O62" s="3">
+      <c r="O62" s="9">
         <v>-90.503845100000007</v>
       </c>
       <c r="P62" s="3">
@@ -5814,7 +5769,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>21</v>
       </c>
@@ -5854,10 +5809,10 @@
       <c r="M63" s="3">
         <v>1</v>
       </c>
-      <c r="N63" s="3">
+      <c r="N63" s="9">
         <v>14.6446387</v>
       </c>
-      <c r="O63" s="3">
+      <c r="O63" s="9">
         <v>-90.512117599999996</v>
       </c>
       <c r="P63" s="3">
@@ -5879,7 +5834,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="64" spans="1:21">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>21</v>
       </c>
@@ -5919,10 +5874,10 @@
       <c r="M64" s="3">
         <v>1</v>
       </c>
-      <c r="N64" s="3">
+      <c r="N64" s="9">
         <v>14.63809</v>
       </c>
-      <c r="O64" s="3">
+      <c r="O64" s="9">
         <v>-90.513705900000005</v>
       </c>
       <c r="P64" s="3">
@@ -5944,7 +5899,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="65" spans="1:21">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>21</v>
       </c>
@@ -5984,10 +5939,10 @@
       <c r="M65" s="3">
         <v>1</v>
       </c>
-      <c r="N65" s="3">
+      <c r="N65" s="9">
         <v>14.628804000000001</v>
       </c>
-      <c r="O65" s="3">
+      <c r="O65" s="9">
         <v>-90.599055300000003</v>
       </c>
       <c r="P65" s="3">
@@ -6009,7 +5964,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="66" spans="1:21">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -6049,10 +6004,10 @@
       <c r="M66" s="3">
         <v>1</v>
       </c>
-      <c r="N66" s="3">
+      <c r="N66" s="9">
         <v>14.644689899999999</v>
       </c>
-      <c r="O66" s="3">
+      <c r="O66" s="9">
         <v>-90.505205200000006</v>
       </c>
       <c r="P66" s="3">
@@ -6074,7 +6029,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="67" spans="1:21">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>21</v>
       </c>
@@ -6114,10 +6069,10 @@
       <c r="M67" s="3">
         <v>9</v>
       </c>
-      <c r="N67" s="3">
+      <c r="N67" s="9">
         <v>14.6068029</v>
       </c>
-      <c r="O67" s="3">
+      <c r="O67" s="9">
         <v>-90.523151200000001</v>
       </c>
       <c r="P67" s="3">
@@ -6139,7 +6094,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="68" spans="1:21">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>21</v>
       </c>
@@ -6179,10 +6134,10 @@
       <c r="M68" s="3">
         <v>12</v>
       </c>
-      <c r="N68" s="3">
+      <c r="N68" s="9">
         <v>14.590601700000001</v>
       </c>
-      <c r="O68" s="3">
+      <c r="O68" s="9">
         <v>-90.560034999999999</v>
       </c>
       <c r="P68" s="3">
@@ -6204,7 +6159,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="69" spans="1:21">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>21</v>
       </c>
@@ -6244,10 +6199,10 @@
       <c r="M69" s="3">
         <v>11</v>
       </c>
-      <c r="N69" s="3">
+      <c r="N69" s="9">
         <v>14.613130699999999</v>
       </c>
-      <c r="O69" s="3">
+      <c r="O69" s="9">
         <v>-90.539060000000006</v>
       </c>
       <c r="P69" s="3">
@@ -6269,7 +6224,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="70" spans="1:21">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>21</v>
       </c>
@@ -6309,10 +6264,10 @@
       <c r="M70" s="3">
         <v>11</v>
       </c>
-      <c r="N70" s="3">
+      <c r="N70" s="9">
         <v>14.600117900000001</v>
       </c>
-      <c r="O70" s="3">
+      <c r="O70" s="9">
         <v>-90.561829000000003</v>
       </c>
       <c r="P70" s="3">
@@ -6334,7 +6289,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="71" spans="1:21">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -6374,10 +6329,10 @@
       <c r="M71" s="3">
         <v>6</v>
       </c>
-      <c r="N71" s="3">
+      <c r="N71" s="9">
         <v>14.662698300000001</v>
       </c>
-      <c r="O71" s="3">
+      <c r="O71" s="9">
         <v>-90.493935899999997</v>
       </c>
       <c r="P71" s="3">
@@ -6399,7 +6354,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="72" spans="1:21">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -6439,10 +6394,10 @@
       <c r="M72" s="3">
         <v>1</v>
       </c>
-      <c r="N72" s="3">
+      <c r="N72" s="9">
         <v>14.6288248</v>
       </c>
-      <c r="O72" s="3">
+      <c r="O72" s="9">
         <v>-90.518449200000006</v>
       </c>
       <c r="P72" s="3">
@@ -6464,7 +6419,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="73" spans="1:21">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -6504,10 +6459,10 @@
       <c r="M73" s="3">
         <v>12</v>
       </c>
-      <c r="N73" s="3">
+      <c r="N73" s="9">
         <v>14.5865425</v>
       </c>
-      <c r="O73" s="3">
+      <c r="O73" s="9">
         <v>-90.541018699999995</v>
       </c>
       <c r="P73" s="3">
@@ -6529,7 +6484,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="74" spans="1:21">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -6569,10 +6524,10 @@
       <c r="M74" s="3">
         <v>0</v>
       </c>
-      <c r="N74" s="3">
+      <c r="N74" s="9">
         <v>14.730167700000001</v>
       </c>
-      <c r="O74" s="3">
+      <c r="O74" s="9">
         <v>-90.635610700000001</v>
       </c>
       <c r="P74" s="3">
@@ -6594,7 +6549,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="75" spans="1:21">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>21</v>
       </c>
@@ -6634,10 +6589,10 @@
       <c r="M75" s="3">
         <v>0</v>
       </c>
-      <c r="N75" s="3">
+      <c r="N75" s="9">
         <v>14.724950099999999</v>
       </c>
-      <c r="O75" s="3">
+      <c r="O75" s="9">
         <v>-90.635651999999993</v>
       </c>
       <c r="P75" s="3">
@@ -6659,7 +6614,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="76" spans="1:21">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -6699,10 +6654,10 @@
       <c r="M76" s="3">
         <v>12</v>
       </c>
-      <c r="N76" s="3">
+      <c r="N76" s="9">
         <v>14.5828878</v>
       </c>
-      <c r="O76" s="3">
+      <c r="O76" s="9">
         <v>-90.565884999999994</v>
       </c>
       <c r="P76" s="3">
@@ -6724,7 +6679,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="77" spans="1:21">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -6764,10 +6719,10 @@
       <c r="M77" s="3">
         <v>11</v>
       </c>
-      <c r="N77" s="3">
+      <c r="N77" s="9">
         <v>14.619236600000001</v>
       </c>
-      <c r="O77" s="3">
+      <c r="O77" s="9">
         <v>-90.553272399999997</v>
       </c>
       <c r="P77" s="3">
@@ -6789,7 +6744,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="78" spans="1:21">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>21</v>
       </c>
@@ -6829,10 +6784,10 @@
       <c r="M78" s="3">
         <v>1</v>
       </c>
-      <c r="N78" s="3">
+      <c r="N78" s="9">
         <v>14.641307100000001</v>
       </c>
-      <c r="O78" s="3">
+      <c r="O78" s="9">
         <v>-90.510813999999996</v>
       </c>
       <c r="P78" s="3">
@@ -6854,7 +6809,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="79" spans="1:21">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>21</v>
       </c>
@@ -6894,10 +6849,10 @@
       <c r="M79" s="3">
         <v>12</v>
       </c>
-      <c r="N79" s="3">
+      <c r="N79" s="9">
         <v>14.566526100000001</v>
       </c>
-      <c r="O79" s="3">
+      <c r="O79" s="9">
         <v>-90.551930600000006</v>
       </c>
       <c r="P79" s="3">
@@ -6919,7 +6874,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="80" spans="1:21">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>21</v>
       </c>
@@ -6959,10 +6914,10 @@
       <c r="M80" s="3">
         <v>1</v>
       </c>
-      <c r="N80" s="3">
+      <c r="N80" s="9">
         <v>14.6396233</v>
       </c>
-      <c r="O80" s="3">
+      <c r="O80" s="9">
         <v>-90.515105800000001</v>
       </c>
       <c r="P80" s="3">
@@ -6984,7 +6939,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="81" spans="1:21">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>21</v>
       </c>
@@ -7024,10 +6979,10 @@
       <c r="M81" s="3">
         <v>6</v>
       </c>
-      <c r="N81" s="3">
+      <c r="N81" s="9">
         <v>14.533012299999999</v>
       </c>
-      <c r="O81" s="3">
+      <c r="O81" s="9">
         <v>-90.584910699999995</v>
       </c>
       <c r="P81" s="3">
@@ -7049,7 +7004,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="82" spans="1:21">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -7089,10 +7044,10 @@
       <c r="M82" s="3">
         <v>10</v>
       </c>
-      <c r="N82" s="3">
+      <c r="N82" s="9">
         <v>14.587255600000001</v>
       </c>
-      <c r="O82" s="3">
+      <c r="O82" s="9">
         <v>-90.501031100000006</v>
       </c>
       <c r="P82" s="3">
@@ -7114,7 +7069,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="83" spans="1:21">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>21</v>
       </c>
@@ -7154,10 +7109,10 @@
       <c r="M83" s="3">
         <v>9</v>
       </c>
-      <c r="N83" s="3">
+      <c r="N83" s="9">
         <v>14.605656400000001</v>
       </c>
-      <c r="O83" s="3">
+      <c r="O83" s="9">
         <v>-90.522127999999995</v>
       </c>
       <c r="P83" s="3">
@@ -7179,7 +7134,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="84" spans="1:21">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>21</v>
       </c>
@@ -7219,10 +7174,10 @@
       <c r="M84" s="3">
         <v>2</v>
       </c>
-      <c r="N84" s="3">
+      <c r="N84" s="9">
         <v>14.6498405</v>
       </c>
-      <c r="O84" s="3">
+      <c r="O84" s="9">
         <v>-90.503781399999994</v>
       </c>
       <c r="P84" s="3">
@@ -7244,7 +7199,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="85" spans="1:21">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>21</v>
       </c>
@@ -7284,10 +7239,10 @@
       <c r="M85" s="3">
         <v>12</v>
       </c>
-      <c r="N85" s="3">
+      <c r="N85" s="9">
         <v>14.5815986</v>
       </c>
-      <c r="O85" s="3">
+      <c r="O85" s="9">
         <v>-90.565893299999999</v>
       </c>
       <c r="P85" s="3">
@@ -7309,7 +7264,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="86" spans="1:21">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>21</v>
       </c>
@@ -7349,10 +7304,10 @@
       <c r="M86" s="3">
         <v>1</v>
       </c>
-      <c r="N86" s="3">
+      <c r="N86" s="9">
         <v>14.6288179</v>
       </c>
-      <c r="O86" s="3">
+      <c r="O86" s="9">
         <v>-90.522310399999995</v>
       </c>
       <c r="P86" s="3">
@@ -7374,7 +7329,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="87" spans="1:21">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>21</v>
       </c>
@@ -7414,10 +7369,10 @@
       <c r="M87" s="3">
         <v>12</v>
       </c>
-      <c r="N87" s="3">
+      <c r="N87" s="9">
         <v>14.5570845</v>
       </c>
-      <c r="O87" s="3">
+      <c r="O87" s="9">
         <v>-90.549368700000002</v>
       </c>
       <c r="P87" s="3">
@@ -7439,7 +7394,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="88" spans="1:21">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -7479,10 +7434,10 @@
       <c r="M88" s="3">
         <v>11</v>
       </c>
-      <c r="N88" s="3">
+      <c r="N88" s="9">
         <v>14.5877143</v>
       </c>
-      <c r="O88" s="3">
+      <c r="O88" s="9">
         <v>-90.562522999999999</v>
       </c>
       <c r="P88" s="3">
@@ -7504,7 +7459,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="89" spans="1:21">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>21</v>
       </c>
@@ -7544,10 +7499,10 @@
       <c r="M89" s="3">
         <v>12</v>
       </c>
-      <c r="N89" s="3">
+      <c r="N89" s="9">
         <v>14.585692099999999</v>
       </c>
-      <c r="O89" s="3">
+      <c r="O89" s="9">
         <v>-90.540455499999993</v>
       </c>
       <c r="P89" s="3">
@@ -7569,7 +7524,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="90" spans="1:21">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>21</v>
       </c>
@@ -7609,10 +7564,10 @@
       <c r="M90" s="3">
         <v>1</v>
       </c>
-      <c r="N90" s="3">
+      <c r="N90" s="9">
         <v>14.535220799999999</v>
       </c>
-      <c r="O90" s="3">
+      <c r="O90" s="9">
         <v>-90.602767900000003</v>
       </c>
       <c r="P90" s="3">
@@ -7634,7 +7589,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="91" spans="1:21">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>21</v>
       </c>
@@ -7674,10 +7629,10 @@
       <c r="M91" s="3">
         <v>0</v>
       </c>
-      <c r="N91" s="3">
+      <c r="N91" s="9">
         <v>14.5127094</v>
       </c>
-      <c r="O91" s="3">
+      <c r="O91" s="9">
         <v>-90.558335600000007</v>
       </c>
       <c r="P91" s="3">
@@ -7699,7 +7654,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="92" spans="1:21">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>21</v>
       </c>
@@ -7739,10 +7694,10 @@
       <c r="M92" s="3">
         <v>12</v>
       </c>
-      <c r="N92" s="3">
+      <c r="N92" s="9">
         <v>14.562232699999999</v>
       </c>
-      <c r="O92" s="3">
+      <c r="O92" s="9">
         <v>-90.549205200000003</v>
       </c>
       <c r="P92" s="3">
@@ -7764,7 +7719,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="93" spans="1:21">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>21</v>
       </c>
@@ -7804,10 +7759,10 @@
       <c r="M93" s="3">
         <v>6</v>
       </c>
-      <c r="N93" s="3">
+      <c r="N93" s="9">
         <v>14.680126899999999</v>
       </c>
-      <c r="O93" s="3">
+      <c r="O93" s="9">
         <v>-90.486313499999994</v>
       </c>
       <c r="P93" s="3">
@@ -7829,7 +7784,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="94" spans="1:21">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>21</v>
       </c>
@@ -7869,10 +7824,10 @@
       <c r="M94" s="3">
         <v>11</v>
       </c>
-      <c r="N94" s="3">
+      <c r="N94" s="9">
         <v>14.5693511</v>
       </c>
-      <c r="O94" s="3">
+      <c r="O94" s="9">
         <v>-90.574008000000006</v>
       </c>
       <c r="P94" s="3">
@@ -7894,7 +7849,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="95" spans="1:21">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>21</v>
       </c>
@@ -7934,10 +7889,10 @@
       <c r="M95" s="3">
         <v>1</v>
       </c>
-      <c r="N95" s="3">
+      <c r="N95" s="9">
         <v>14.6355474</v>
       </c>
-      <c r="O95" s="3">
+      <c r="O95" s="9">
         <v>-90.521380899999997</v>
       </c>
       <c r="P95" s="3">
@@ -7959,7 +7914,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="96" spans="1:21">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>21</v>
       </c>
@@ -7999,10 +7954,10 @@
       <c r="M96" s="3">
         <v>12</v>
       </c>
-      <c r="N96" s="3">
+      <c r="N96" s="9">
         <v>14.5776295</v>
       </c>
-      <c r="O96" s="3">
+      <c r="O96" s="9">
         <v>-90.546588099999994</v>
       </c>
       <c r="P96" s="3">
@@ -8024,7 +7979,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="97" spans="1:21">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>21</v>
       </c>
@@ -8064,10 +8019,10 @@
       <c r="M97" s="3">
         <v>1</v>
       </c>
-      <c r="N97" s="3">
+      <c r="N97" s="9">
         <v>14.6314782</v>
       </c>
-      <c r="O97" s="3">
+      <c r="O97" s="9">
         <v>-90.513215799999998</v>
       </c>
       <c r="P97" s="3">
@@ -8089,7 +8044,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="98" spans="1:21">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>21</v>
       </c>
@@ -8129,10 +8084,10 @@
       <c r="M98" s="3">
         <v>7</v>
       </c>
-      <c r="N98" s="3">
+      <c r="N98" s="9">
         <v>14.6380485</v>
       </c>
-      <c r="O98" s="3">
+      <c r="O98" s="9">
         <v>-90.603833699999996</v>
       </c>
       <c r="P98" s="3">
@@ -8154,7 +8109,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="99" spans="1:21">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>21</v>
       </c>
@@ -8194,10 +8149,10 @@
       <c r="M99" s="3">
         <v>8</v>
       </c>
-      <c r="N99" s="3">
+      <c r="N99" s="9">
         <v>14.6546675</v>
       </c>
-      <c r="O99" s="3">
+      <c r="O99" s="9">
         <v>-90.594201200000001</v>
       </c>
       <c r="P99" s="3">
@@ -8219,7 +8174,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="100" spans="1:21">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>21</v>
       </c>
@@ -8259,10 +8214,10 @@
       <c r="M100" s="3">
         <v>0</v>
       </c>
-      <c r="N100" s="3">
+      <c r="N100" s="9">
         <v>14.470166600000001</v>
       </c>
-      <c r="O100" s="3">
+      <c r="O100" s="9">
         <v>-90.631758700000006</v>
       </c>
       <c r="P100" s="3">
@@ -8284,7 +8239,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="101" spans="1:21">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>21</v>
       </c>
@@ -8324,10 +8279,10 @@
       <c r="M101" s="3">
         <v>1</v>
       </c>
-      <c r="N101" s="3">
+      <c r="N101" s="9">
         <v>14.6334672</v>
       </c>
-      <c r="O101" s="3">
+      <c r="O101" s="9">
         <v>-90.515145700000005</v>
       </c>
       <c r="P101" s="3">
@@ -8349,7 +8304,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="102" spans="1:21">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -8389,10 +8344,10 @@
       <c r="M102" s="3">
         <v>12</v>
       </c>
-      <c r="N102" s="3">
+      <c r="N102" s="9">
         <v>14.5638799</v>
       </c>
-      <c r="O102" s="3">
+      <c r="O102" s="9">
         <v>-90.552602399999998</v>
       </c>
       <c r="P102" s="3">
@@ -8414,7 +8369,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="103" spans="1:21">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>21</v>
       </c>
@@ -8454,10 +8409,10 @@
       <c r="M103" s="3">
         <v>5</v>
       </c>
-      <c r="N103" s="3">
+      <c r="N103" s="9">
         <v>14.617900799999999</v>
       </c>
-      <c r="O103" s="3">
+      <c r="O103" s="9">
         <v>-90.512985099999995</v>
       </c>
       <c r="P103" s="3">
@@ -8479,7 +8434,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="104" spans="1:21">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>21</v>
       </c>
@@ -8519,10 +8474,10 @@
       <c r="M104" s="3">
         <v>12</v>
       </c>
-      <c r="N104" s="3">
+      <c r="N104" s="9">
         <v>14.5953078</v>
       </c>
-      <c r="O104" s="3">
+      <c r="O104" s="9">
         <v>-90.544155799999999</v>
       </c>
       <c r="P104" s="3">
@@ -8544,7 +8499,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="105" spans="1:21">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>21</v>
       </c>
@@ -8584,10 +8539,10 @@
       <c r="M105" s="3">
         <v>10</v>
       </c>
-      <c r="N105" s="3">
+      <c r="N105" s="9">
         <v>14.5987808</v>
       </c>
-      <c r="O105" s="3">
+      <c r="O105" s="9">
         <v>-90.510694099999995</v>
       </c>
       <c r="P105" s="3">
@@ -8609,7 +8564,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="106" spans="1:21">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>21</v>
       </c>
@@ -8649,10 +8604,10 @@
       <c r="M106" s="3">
         <v>12</v>
       </c>
-      <c r="N106" s="3">
+      <c r="N106" s="9">
         <v>14.564778199999999</v>
       </c>
-      <c r="O106" s="3">
+      <c r="O106" s="9">
         <v>-90.575215099999994</v>
       </c>
       <c r="P106" s="3">
@@ -8674,7 +8629,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="107" spans="1:21">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>21</v>
       </c>
@@ -8714,10 +8669,10 @@
       <c r="M107" s="3">
         <v>12</v>
       </c>
-      <c r="N107" s="3">
+      <c r="N107" s="9">
         <v>14.565428300000001</v>
       </c>
-      <c r="O107" s="3">
+      <c r="O107" s="9">
         <v>-90.549242199999995</v>
       </c>
       <c r="P107" s="3">
@@ -8739,7 +8694,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="108" spans="1:21">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>21</v>
       </c>
@@ -8779,10 +8734,10 @@
       <c r="M108" s="3">
         <v>10</v>
       </c>
-      <c r="N108" s="3">
+      <c r="N108" s="9">
         <v>14.5989416</v>
       </c>
-      <c r="O108" s="3">
+      <c r="O108" s="9">
         <v>-90.510794300000001</v>
       </c>
       <c r="P108" s="3">
@@ -8804,7 +8759,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="109" spans="1:21">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>21</v>
       </c>
@@ -8844,10 +8799,10 @@
       <c r="M109" s="3">
         <v>10</v>
       </c>
-      <c r="N109" s="3">
+      <c r="N109" s="9">
         <v>14.5946499</v>
       </c>
-      <c r="O109" s="3">
+      <c r="O109" s="9">
         <v>-90.516454199999998</v>
       </c>
       <c r="P109" s="3">
@@ -8869,7 +8824,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="110" spans="1:21">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>21</v>
       </c>
@@ -8909,10 +8864,10 @@
       <c r="M110" s="3">
         <v>10</v>
       </c>
-      <c r="N110" s="3">
+      <c r="N110" s="9">
         <v>14.595564100000001</v>
       </c>
-      <c r="O110" s="3">
+      <c r="O110" s="9">
         <v>-90.515670900000003</v>
       </c>
       <c r="P110" s="3">
@@ -8934,7 +8889,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="111" spans="1:21">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>21</v>
       </c>
@@ -8962,22 +8917,22 @@
       <c r="I111" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="J111" s="7" t="s">
+      <c r="J111" s="7">
+        <v>10103122</v>
+      </c>
+      <c r="K111" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="K111" s="7" t="s">
+      <c r="L111" s="7" t="s">
         <v>379</v>
-      </c>
-      <c r="L111" s="7" t="s">
-        <v>380</v>
       </c>
       <c r="M111" s="7">
         <v>3</v>
       </c>
-      <c r="N111" s="7">
+      <c r="N111" s="10">
         <v>14.6152278</v>
       </c>
-      <c r="O111" s="7">
+      <c r="O111" s="10">
         <v>-90.532918899999999</v>
       </c>
       <c r="P111" s="2"/>
@@ -8989,13 +8944,13 @@
         <v>45040.426718518524</v>
       </c>
       <c r="T111" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U111" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="112" spans="1:21">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>21</v>
       </c>
@@ -9023,22 +8978,22 @@
       <c r="I112" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="J112" s="7" t="s">
+      <c r="J112" s="7">
+        <v>10101113</v>
+      </c>
+      <c r="K112" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="L112" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="K112" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="L112" s="7" t="s">
-        <v>384</v>
-      </c>
       <c r="M112" s="7">
         <v>1</v>
       </c>
-      <c r="N112" s="7">
+      <c r="N112" s="10">
         <v>14.640407400000001</v>
       </c>
-      <c r="O112" s="7">
+      <c r="O112" s="10">
         <v>-90.508473100000003</v>
       </c>
       <c r="P112" s="2"/>
@@ -9050,13 +9005,13 @@
         <v>45030.4079399537</v>
       </c>
       <c r="T112" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U112" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="113" spans="1:21">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>21</v>
       </c>
@@ -9079,27 +9034,27 @@
         <v>71</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="J113" s="7" t="s">
-        <v>386</v>
+      <c r="J113" s="7">
+        <v>10101011</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="L113" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="M113" s="7">
         <v>1</v>
       </c>
-      <c r="N113" s="7">
+      <c r="N113" s="10">
         <v>14.6429043</v>
       </c>
-      <c r="O113" s="7">
+      <c r="O113" s="10">
         <v>-90.511481000000003</v>
       </c>
       <c r="P113" s="2"/>
@@ -9111,13 +9066,13 @@
         <v>45012.616581817128</v>
       </c>
       <c r="T113" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U113" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="114" spans="1:21">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>21</v>
       </c>
@@ -9145,22 +9100,22 @@
       <c r="I114" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J114" s="7" t="s">
-        <v>390</v>
+      <c r="J114" s="7">
+        <v>10101073</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="L114" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="M114" s="7">
         <v>1</v>
       </c>
-      <c r="N114" s="7">
+      <c r="N114" s="10">
         <v>14.631730599999999</v>
       </c>
-      <c r="O114" s="7">
+      <c r="O114" s="10">
         <v>-90.516235600000002</v>
       </c>
       <c r="P114" s="2"/>
@@ -9172,13 +9127,13 @@
         <v>45000.438891516213</v>
       </c>
       <c r="T114" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U114" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="115" spans="1:21">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>21</v>
       </c>
@@ -9201,27 +9156,27 @@
         <v>0</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="J115" s="7" t="s">
-        <v>395</v>
+        <v>390</v>
+      </c>
+      <c r="J115" s="7">
+        <v>10104124</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="L115" s="7" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="M115" s="7">
         <v>4</v>
       </c>
-      <c r="N115" s="7">
+      <c r="N115" s="10">
         <v>14.625111</v>
       </c>
-      <c r="O115" s="7">
+      <c r="O115" s="10">
         <v>-90.516414699999999</v>
       </c>
       <c r="P115" s="2"/>
@@ -9233,13 +9188,13 @@
         <v>45036.414814189811</v>
       </c>
       <c r="T115" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U115" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="116" spans="1:21">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>21</v>
       </c>
@@ -9267,22 +9222,22 @@
       <c r="I116" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="J116" s="7" t="s">
-        <v>398</v>
+      <c r="J116" s="7">
+        <v>10101120</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="L116" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="M116" s="7">
         <v>1</v>
       </c>
-      <c r="N116" s="7">
+      <c r="N116" s="10">
         <v>14.6283589</v>
       </c>
-      <c r="O116" s="7">
+      <c r="O116" s="10">
         <v>-90.509923499999999</v>
       </c>
       <c r="P116" s="2"/>
@@ -9294,13 +9249,13 @@
         <v>45040.522242615742</v>
       </c>
       <c r="T116" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U116" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="117" spans="1:21">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>21</v>
       </c>
@@ -9326,24 +9281,24 @@
         <v>38</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="J117" s="7" t="s">
-        <v>401</v>
+        <v>390</v>
+      </c>
+      <c r="J117" s="7">
+        <v>10101100</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="L117" s="7" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="M117" s="7">
         <v>1</v>
       </c>
-      <c r="N117" s="7">
+      <c r="N117" s="10">
         <v>14.6413183</v>
       </c>
-      <c r="O117" s="7">
+      <c r="O117" s="10">
         <v>-90.510794500000003</v>
       </c>
       <c r="P117" s="2"/>
@@ -9355,13 +9310,13 @@
         <v>45034.589677152777</v>
       </c>
       <c r="T117" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U117" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="118" spans="1:21">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>21</v>
       </c>
@@ -9389,22 +9344,22 @@
       <c r="I118" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="J118" s="7" t="s">
-        <v>404</v>
+      <c r="J118" s="7">
+        <v>10111036</v>
       </c>
       <c r="K118" s="7" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="L118" s="7" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="M118" s="7">
         <v>10</v>
       </c>
-      <c r="N118" s="7">
+      <c r="N118" s="10">
         <v>14.6380479</v>
       </c>
-      <c r="O118" s="7">
+      <c r="O118" s="10">
         <v>-90.604205800000003</v>
       </c>
       <c r="P118" s="2"/>
@@ -9416,13 +9371,13 @@
         <v>44987.405489513891</v>
       </c>
       <c r="T118" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U118" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="119" spans="1:21">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>21</v>
       </c>
@@ -9450,22 +9405,22 @@
       <c r="I119" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="J119" s="7" t="s">
-        <v>407</v>
+      <c r="J119" s="7">
+        <v>10101115</v>
       </c>
       <c r="K119" s="7" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="L119" s="7" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="M119" s="7">
         <v>11</v>
       </c>
-      <c r="N119" s="7">
+      <c r="N119" s="10">
         <v>14.6142907</v>
       </c>
-      <c r="O119" s="7">
+      <c r="O119" s="10">
         <v>-90.5393021</v>
       </c>
       <c r="P119" s="2"/>
@@ -9477,13 +9432,13 @@
         <v>44991.485673877323</v>
       </c>
       <c r="T119" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U119" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="120" spans="1:21">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>21</v>
       </c>
@@ -9506,27 +9461,27 @@
         <v>111</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="I120" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J120" s="7" t="s">
-        <v>411</v>
+      <c r="J120" s="7">
+        <v>10106118</v>
       </c>
       <c r="K120" s="7" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="L120" s="7" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="M120" s="7">
         <v>6</v>
       </c>
-      <c r="N120" s="7">
+      <c r="N120" s="10">
         <v>14.650486799999999</v>
       </c>
-      <c r="O120" s="7">
+      <c r="O120" s="10">
         <v>-90.497748000000001</v>
       </c>
       <c r="P120" s="2"/>
@@ -9538,13 +9493,13 @@
         <v>44988.6408537963</v>
       </c>
       <c r="T120" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U120" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="121" spans="1:21">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>21</v>
       </c>
@@ -9570,24 +9525,24 @@
         <v>80</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="J121" s="9" t="s">
-        <v>415</v>
+        <v>404</v>
+      </c>
+      <c r="J121" s="7">
+        <v>10101061</v>
       </c>
       <c r="K121" s="7" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="L121" s="7" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="M121" s="7">
         <v>1</v>
       </c>
-      <c r="N121" s="7">
+      <c r="N121" s="10">
         <v>14.6443625</v>
       </c>
-      <c r="O121" s="7">
+      <c r="O121" s="10">
         <v>-90.504285499999995</v>
       </c>
       <c r="P121" s="2"/>
@@ -9599,13 +9554,13 @@
         <v>45033.501822442129</v>
       </c>
       <c r="T121" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U121" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="122" spans="1:21">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>21</v>
       </c>
@@ -9633,22 +9588,22 @@
       <c r="I122" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J122" s="7" t="s">
-        <v>418</v>
+      <c r="J122" s="7">
+        <v>10101114</v>
       </c>
       <c r="K122" s="7" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="L122" s="7" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="M122" s="7">
         <v>1</v>
       </c>
-      <c r="N122" s="7">
+      <c r="N122" s="10">
         <v>14.6427423</v>
       </c>
-      <c r="O122" s="7">
+      <c r="O122" s="10">
         <v>-90.509433599999994</v>
       </c>
       <c r="P122" s="2"/>
@@ -9660,13 +9615,13 @@
         <v>45008.477398877323</v>
       </c>
       <c r="T122" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U122" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="123" spans="1:21">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>21</v>
       </c>
@@ -9694,22 +9649,22 @@
       <c r="I123" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J123" s="7" t="s">
-        <v>421</v>
+      <c r="J123" s="7">
+        <v>10101112</v>
       </c>
       <c r="K123" s="7" t="s">
         <v>98</v>
       </c>
       <c r="L123" s="7" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="M123" s="7">
         <v>1</v>
       </c>
-      <c r="N123" s="7">
+      <c r="N123" s="10">
         <v>14.6374546</v>
       </c>
-      <c r="O123" s="7">
+      <c r="O123" s="10">
         <v>-90.512252899999993</v>
       </c>
       <c r="P123" s="2"/>
@@ -9721,13 +9676,13 @@
         <v>45030.453880486108</v>
       </c>
       <c r="T123" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U123" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="124" spans="1:21">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>21</v>
       </c>
@@ -9750,27 +9705,27 @@
         <v>115</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="I124" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="J124" s="7" t="s">
-        <v>424</v>
+        <v>390</v>
+      </c>
+      <c r="J124" s="7">
+        <v>10117123</v>
       </c>
       <c r="K124" s="7" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="L124" s="7" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="M124" s="7">
         <v>17</v>
       </c>
-      <c r="N124" s="7">
+      <c r="N124" s="10">
         <v>14.647081699999999</v>
       </c>
-      <c r="O124" s="7">
+      <c r="O124" s="10">
         <v>-90.477213800000001</v>
       </c>
       <c r="P124" s="2"/>
@@ -9782,13 +9737,13 @@
         <v>44998.40762179398</v>
       </c>
       <c r="T124" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U124" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="125" spans="1:21">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>21</v>
       </c>
@@ -9816,11 +9771,11 @@
       <c r="I125" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J125" s="7" t="s">
-        <v>427</v>
+      <c r="J125" s="7">
+        <v>10101027</v>
       </c>
       <c r="K125" s="7" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="L125" s="7" t="s">
         <v>37</v>
@@ -9828,10 +9783,10 @@
       <c r="M125" s="7">
         <v>1</v>
       </c>
-      <c r="N125" s="7">
+      <c r="N125" s="10">
         <v>14.6289614</v>
       </c>
-      <c r="O125" s="7">
+      <c r="O125" s="10">
         <v>-90.518420800000001</v>
       </c>
       <c r="P125" s="2"/>
@@ -9843,13 +9798,13 @@
         <v>44986.473184050927</v>
       </c>
       <c r="T125" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U125" s="3">
         <v>2023</v>
       </c>
     </row>
-    <row r="126" spans="1:21">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>21</v>
       </c>
@@ -9877,22 +9832,22 @@
       <c r="I126" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="J126" s="7" t="s">
-        <v>429</v>
+      <c r="J126" s="7">
+        <v>10101116</v>
       </c>
       <c r="K126" s="7" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="L126" s="7" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="M126" s="7">
         <v>1</v>
       </c>
-      <c r="N126" s="7">
+      <c r="N126" s="10">
         <v>14.630362399999999</v>
       </c>
-      <c r="O126" s="7">
+      <c r="O126" s="10">
         <v>-90.519656600000005</v>
       </c>
       <c r="P126" s="2"/>
@@ -9904,7 +9859,7 @@
         <v>45036.512567812497</v>
       </c>
       <c r="T126" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U126" s="3">
         <v>2023</v>

</xml_diff>